<commit_message>
Updated the battery charge.
</commit_message>
<xml_diff>
--- a/Schematics/Batteri.xlsx
+++ b/Schematics/Batteri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\mini-el-ECU\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C42D46E-5C03-4052-B6DC-5581683D743D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933E06B2-A04F-4270-B2E3-46914EC210CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{31926B73-E62F-4486-9E6A-C8E33EA3A9BF}"/>
   </bookViews>
@@ -211,30 +211,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$3</c:f>
+              <c:f>Batterimåling!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>45660</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$B$2:$B$3</c:f>
+              <c:f>Batterimåling!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>10.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,30 +280,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$3</c:f>
+              <c:f>Batterimåling!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>45660</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$C$2:$C$3</c:f>
+              <c:f>Batterimåling!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>10.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,30 +349,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$3</c:f>
+              <c:f>Batterimåling!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>45660</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$D$2:$D$3</c:f>
+              <c:f>Batterimåling!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>12.76</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,30 +418,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$3</c:f>
+              <c:f>Batterimåling!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>45660</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$E$2:$E$3</c:f>
+              <c:f>Batterimåling!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>12.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAAE12D-6070-4A73-969C-5B5B0E707FB0}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,6 +1617,23 @@
         <v>12.3</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45661</v>
+      </c>
+      <c r="B4">
+        <v>12.31</v>
+      </c>
+      <c r="C4">
+        <v>11.8</v>
+      </c>
+      <c r="D4">
+        <v>12.84</v>
+      </c>
+      <c r="E4" s="2">
+        <v>13.12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Battery voltages after a couple of rest days.
</commit_message>
<xml_diff>
--- a/Schematics/Batteri.xlsx
+++ b/Schematics/Batteri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\mini-el-ECU\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933E06B2-A04F-4270-B2E3-46914EC210CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79D08DF-8481-418D-8855-4B01CE1BA136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{31926B73-E62F-4486-9E6A-C8E33EA3A9BF}"/>
   </bookViews>
@@ -211,10 +211,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$4</c:f>
+              <c:f>Batterimåling!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -223,16 +223,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$B$2:$B$4</c:f>
+              <c:f>Batterimåling!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10.45</c:v>
                 </c:pt>
@@ -241,6 +247,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,10 +292,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$4</c:f>
+              <c:f>Batterimåling!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -292,24 +304,36 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$C$2:$C$4</c:f>
+              <c:f>Batterimåling!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>10.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.55</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="0.00">
                   <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.61</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>12.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -349,10 +373,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$4</c:f>
+              <c:f>Batterimåling!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -361,16 +385,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$D$2:$D$4</c:f>
+              <c:f>Batterimåling!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>12.76</c:v>
                 </c:pt>
@@ -379,6 +409,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,10 +454,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$4</c:f>
+              <c:f>Batterimåling!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -430,16 +466,22 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$E$2:$E$4</c:f>
+              <c:f>Batterimåling!$E$2:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>12.45</c:v>
                 </c:pt>
@@ -448,6 +490,12 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>13.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,7 +1277,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1555,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAAE12D-6070-4A73-969C-5B5B0E707FB0}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,7 +1672,7 @@
       <c r="B4">
         <v>12.31</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>11.8</v>
       </c>
       <c r="D4">
@@ -1632,6 +1680,40 @@
       </c>
       <c r="E4" s="2">
         <v>13.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45662</v>
+      </c>
+      <c r="B5">
+        <v>12.76</v>
+      </c>
+      <c r="C5">
+        <v>12.61</v>
+      </c>
+      <c r="D5">
+        <v>12.94</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45664</v>
+      </c>
+      <c r="B6">
+        <v>12.54</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="D6">
+        <v>12.68</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Battery voltage after another rest day.
Chargers applied, XS3600 @ #B
</commit_message>
<xml_diff>
--- a/Schematics/Batteri.xlsx
+++ b/Schematics/Batteri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\mini-el-ECU\Schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79D08DF-8481-418D-8855-4B01CE1BA136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0206CC96-BCBE-419F-9CC9-5C6DE5B6E1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{31926B73-E62F-4486-9E6A-C8E33EA3A9BF}"/>
   </bookViews>
@@ -211,10 +211,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$6</c:f>
+              <c:f>Batterimåling!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -229,16 +229,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$B$2:$B$6</c:f>
+              <c:f>Batterimåling!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>10.45</c:v>
                 </c:pt>
@@ -253,6 +256,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.47</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,10 +298,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$6</c:f>
+              <c:f>Batterimåling!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -310,16 +316,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$C$2:$C$6</c:f>
+              <c:f>Batterimåling!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>10.09</c:v>
                 </c:pt>
@@ -334,6 +343,9 @@
                 </c:pt>
                 <c:pt idx="4" formatCode="0.00">
                   <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>12.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -373,10 +385,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$6</c:f>
+              <c:f>Batterimåling!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -391,16 +403,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$D$2:$D$6</c:f>
+              <c:f>Batterimåling!$D$2:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>12.76</c:v>
                 </c:pt>
@@ -415,6 +430,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,10 +472,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Batterimåling!$A$2:$A$6</c:f>
+              <c:f>Batterimåling!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45659</c:v>
                 </c:pt>
@@ -472,16 +490,19 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Batterimåling!$E$2:$E$6</c:f>
+              <c:f>Batterimåling!$E$2:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>12.45</c:v>
                 </c:pt>
@@ -496,6 +517,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>12.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,7 +597,7 @@
         <c:axId val="1009664640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6"/>
+          <c:min val="8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1277,8 +1301,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1603,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAAE12D-6070-4A73-969C-5B5B0E707FB0}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1716,6 +1740,23 @@
         <v>12.27</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45665</v>
+      </c>
+      <c r="B7">
+        <v>12.47</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12.18</v>
+      </c>
+      <c r="D7">
+        <v>12.72</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12.32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>